<commit_message>
update guest method implemented and tested
</commit_message>
<xml_diff>
--- a/routes_design.xlsx
+++ b/routes_design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rumble/Documents/WeddingSongRequest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{70A44B94-A891-7F49-BD50-40858333825C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB4468BD-77B6-D54B-AC5D-1B6118EFD772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15800" xr2:uid="{D98520DE-90ED-1842-9CAD-02F5B5F8C61E}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="68">
   <si>
     <t>Route</t>
   </si>
@@ -182,6 +182,311 @@
       </rPr>
       <t xml:space="preserve"> (email verification token)</t>
     </r>
+  </si>
+  <si>
+    <t>/guests</t>
+  </si>
+  <si>
+    <t>Get a list of all guests</t>
+  </si>
+  <si>
+    <t>JSON array of guest objects</t>
+  </si>
+  <si>
+    <t>/guests/{id}</t>
+  </si>
+  <si>
+    <t>Get details of a specific guest</t>
+  </si>
+  <si>
+    <r>
+      <t>id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (integer)</t>
+    </r>
+  </si>
+  <si>
+    <t>JSON object with guest details</t>
+  </si>
+  <si>
+    <t>Add a new guest</t>
+  </si>
+  <si>
+    <r>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>email</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>password</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>oauth_provider</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>oauth_provider_id</t>
+    </r>
+  </si>
+  <si>
+    <t>JSON object with created guest info</t>
+  </si>
+  <si>
+    <t>Update an existing guest</t>
+  </si>
+  <si>
+    <r>
+      <t>id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (integer), </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>email</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>password</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>oauth_provider</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>oauth_provider_id</t>
+    </r>
+  </si>
+  <si>
+    <t>JSON object with updated guest info</t>
+  </si>
+  <si>
+    <t>Delete a specific guest</t>
+  </si>
+  <si>
+    <t>Success message or status code</t>
+  </si>
+  <si>
+    <t>/guests/search</t>
+  </si>
+  <si>
+    <t>Search guests by criteria</t>
+  </si>
+  <si>
+    <r>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>email</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>oauth_provider</t>
+    </r>
+  </si>
+  <si>
+    <t>JSON array of matching guest objects</t>
+  </si>
+  <si>
+    <t>/guests/{id}/history</t>
+  </si>
+  <si>
+    <t>Get history of interactions for a guest</t>
+  </si>
+  <si>
+    <t>JSON array of interactions (if applicable)</t>
+  </si>
+  <si>
+    <t>/guests/{id}/events</t>
+  </si>
+  <si>
+    <t>Get events related to a guest</t>
+  </si>
+  <si>
+    <t>JSON array of events (if applicable)</t>
+  </si>
+  <si>
+    <t>GUESTS</t>
   </si>
 </sst>
 </file>
@@ -283,7 +588,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -309,6 +614,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -624,16 +950,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE3873A4-E976-7D46-8E74-B618A7E6E516}">
-  <dimension ref="B2:G23"/>
+  <dimension ref="B2:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="27.1640625" customWidth="1"/>
-    <col min="4" max="4" width="18.5" customWidth="1"/>
+    <col min="4" max="4" width="24" customWidth="1"/>
     <col min="5" max="5" width="27.6640625" customWidth="1"/>
     <col min="6" max="6" width="26" customWidth="1"/>
     <col min="7" max="7" width="21" customWidth="1"/>
@@ -800,12 +1126,12 @@
       </c>
     </row>
     <row r="16" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B17" s="7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>0</v>
       </c>
@@ -825,7 +1151,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>18</v>
       </c>
@@ -843,7 +1169,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="2:7" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
         <v>18</v>
       </c>
@@ -861,7 +1187,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="2:7" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
         <v>25</v>
       </c>
@@ -879,7 +1205,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
         <v>25</v>
       </c>
@@ -897,7 +1223,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
         <v>25</v>
       </c>
@@ -913,6 +1239,184 @@
       </c>
       <c r="G23" s="4" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="2:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="16" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H27" s="10"/>
+    </row>
+    <row r="28" spans="2:8" ht="36" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="15"/>
+      <c r="E28" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F28" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="H28" s="10"/>
+    </row>
+    <row r="29" spans="2:8" ht="36" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="13"/>
+      <c r="E29" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F29" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="G29" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="H29" s="10"/>
+    </row>
+    <row r="30" spans="2:8" ht="54" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D30" s="13"/>
+      <c r="E30" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="F30" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="G30" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="H30" s="10"/>
+    </row>
+    <row r="31" spans="2:8" ht="54" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D31" s="13"/>
+      <c r="E31" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="F31" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="G31" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="H31" s="10"/>
+    </row>
+    <row r="32" spans="2:8" ht="36" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D32" s="13"/>
+      <c r="E32" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="F32" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="G32" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="H32" s="10"/>
+    </row>
+    <row r="33" spans="2:8" ht="36" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" s="13"/>
+      <c r="E33" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="F33" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="G33" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="H33" s="10"/>
+    </row>
+    <row r="34" spans="2:8" ht="53" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" s="13"/>
+      <c r="E34" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="F34" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="G34" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="H34" s="10"/>
+    </row>
+    <row r="35" spans="2:8" ht="36" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35" s="13"/>
+      <c r="E35" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="F35" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="G35" s="11" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Event Routes TDD's and working
</commit_message>
<xml_diff>
--- a/routes_design.xlsx
+++ b/routes_design.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rumble/Documents/WeddingSongRequest/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rumble/Documents/WeddingRequester/Function-Band-Request-a-Song-App/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB4468BD-77B6-D54B-AC5D-1B6118EFD772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDAB5425-3EB6-2449-9B3B-748D4D48FDA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15800" xr2:uid="{D98520DE-90ED-1842-9CAD-02F5B5F8C61E}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="78">
   <si>
     <t>Route</t>
   </si>
@@ -487,6 +487,36 @@
   </si>
   <si>
     <t>GUESTS</t>
+  </si>
+  <si>
+    <t>BANDS</t>
+  </si>
+  <si>
+    <t>/bands</t>
+  </si>
+  <si>
+    <t>/bands/{id}</t>
+  </si>
+  <si>
+    <t>/bands/search</t>
+  </si>
+  <si>
+    <t>/bands/{id}/history</t>
+  </si>
+  <si>
+    <t>/bands/{id}/events</t>
+  </si>
+  <si>
+    <t>Get events by band ID</t>
+  </si>
+  <si>
+    <t>band_id</t>
+  </si>
+  <si>
+    <t>JSON(list of events for the band)</t>
+  </si>
+  <si>
+    <t>/events/band_id/events</t>
   </si>
 </sst>
 </file>
@@ -516,12 +546,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="5">
@@ -588,14 +624,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -627,15 +657,38 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -950,10 +1003,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE3873A4-E976-7D46-8E74-B618A7E6E516}">
-  <dimension ref="B2:H35"/>
+  <dimension ref="B2:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -962,460 +1015,648 @@
     <col min="4" max="4" width="24" customWidth="1"/>
     <col min="5" max="5" width="27.6640625" customWidth="1"/>
     <col min="6" max="6" width="26" customWidth="1"/>
-    <col min="7" max="7" width="21" customWidth="1"/>
+    <col min="7" max="7" width="30.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4" t="s">
+      <c r="D5" s="2"/>
+      <c r="E5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4" t="s">
+      <c r="D10" s="2"/>
+      <c r="E10" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4" t="s">
+      <c r="D11" s="2"/>
+      <c r="E11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G11" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4" t="s">
+      <c r="D12" s="2"/>
+      <c r="E12" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="G12" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="2:7" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4" t="s">
+      <c r="D13" s="2"/>
+      <c r="E13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="G13" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="14" spans="2:7" ht="36" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4" t="s">
+      <c r="D14" s="2"/>
+      <c r="E14" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="F14" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="G14" s="9" t="s">
+      <c r="G14" s="7" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="16" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="17" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="5" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E18" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="F18" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G18" s="6" t="s">
+      <c r="G18" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="19" spans="2:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2" t="s">
+      <c r="D19" s="19"/>
+      <c r="E19" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="F19" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="G19" s="19" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="20" spans="2:8" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4" t="s">
+      <c r="D20" s="21"/>
+      <c r="E20" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="4" t="s">
+      <c r="F20" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="G20" s="4" t="s">
+      <c r="G20" s="21" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="21" spans="2:8" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4" t="s">
+      <c r="D21" s="21"/>
+      <c r="E21" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="F21" s="4" t="s">
+      <c r="F21" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="G21" s="4" t="s">
+      <c r="G21" s="21" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="22" spans="2:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4" t="s">
+      <c r="D22" s="21"/>
+      <c r="E22" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="F22" s="4" t="s">
+      <c r="F22" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="G22" s="4" t="s">
+      <c r="G22" s="21" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="23" spans="2:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4" t="s">
+      <c r="D23" s="21"/>
+      <c r="E23" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="F23" s="4" t="s">
+      <c r="F23" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="G23" s="4" t="s">
+      <c r="G23" s="21" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="22"/>
+      <c r="E24" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="F24" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="G24" s="23" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="25" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="26" spans="2:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="16" t="s">
+      <c r="B26" s="3" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="27" spans="2:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D27" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E27" s="6" t="s">
+      <c r="E27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F27" s="6" t="s">
+      <c r="F27" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G27" s="6" t="s">
+      <c r="G27" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H27" s="10"/>
+      <c r="H27" s="8"/>
     </row>
     <row r="28" spans="2:8" ht="36" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="14" t="s">
+      <c r="B28" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="C28" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D28" s="15"/>
-      <c r="E28" s="9" t="s">
+      <c r="D28" s="14"/>
+      <c r="E28" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="F28" s="15" t="s">
+      <c r="F28" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="G28" s="9" t="s">
+      <c r="G28" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="H28" s="10"/>
+      <c r="H28" s="8"/>
     </row>
     <row r="29" spans="2:8" ht="36" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="12" t="s">
+      <c r="B29" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="C29" s="11" t="s">
+      <c r="C29" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D29" s="13"/>
-      <c r="E29" s="11" t="s">
+      <c r="D29" s="11"/>
+      <c r="E29" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F29" s="13" t="s">
+      <c r="F29" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="G29" s="11" t="s">
+      <c r="G29" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="H29" s="10"/>
+      <c r="H29" s="8"/>
     </row>
     <row r="30" spans="2:8" ht="54" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="12" t="s">
+      <c r="B30" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="C30" s="11" t="s">
+      <c r="C30" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D30" s="13"/>
-      <c r="E30" s="11" t="s">
+      <c r="D30" s="17"/>
+      <c r="E30" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="F30" s="13" t="s">
+      <c r="F30" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="G30" s="11" t="s">
+      <c r="G30" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="H30" s="10"/>
+      <c r="H30" s="8"/>
     </row>
     <row r="31" spans="2:8" ht="54" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="12" t="s">
+      <c r="B31" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="C31" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D31" s="13"/>
-      <c r="E31" s="11" t="s">
+      <c r="D31" s="11"/>
+      <c r="E31" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="F31" s="13" t="s">
+      <c r="F31" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="G31" s="11" t="s">
+      <c r="G31" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="H31" s="10"/>
+      <c r="H31" s="8"/>
     </row>
     <row r="32" spans="2:8" ht="36" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="12" t="s">
+      <c r="B32" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="C32" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D32" s="13"/>
-      <c r="E32" s="11" t="s">
+      <c r="D32" s="11"/>
+      <c r="E32" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="F32" s="13" t="s">
+      <c r="F32" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="G32" s="11" t="s">
+      <c r="G32" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="H32" s="10"/>
+      <c r="H32" s="8"/>
     </row>
     <row r="33" spans="2:8" ht="36" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="12" t="s">
+      <c r="B33" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C33" s="11" t="s">
+      <c r="C33" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D33" s="13"/>
-      <c r="E33" s="11" t="s">
+      <c r="D33" s="11"/>
+      <c r="E33" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="F33" s="13" t="s">
+      <c r="F33" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="G33" s="11" t="s">
+      <c r="G33" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="H33" s="10"/>
+      <c r="H33" s="8"/>
     </row>
     <row r="34" spans="2:8" ht="53" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="12" t="s">
+      <c r="B34" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="C34" s="11" t="s">
+      <c r="C34" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D34" s="13"/>
-      <c r="E34" s="11" t="s">
+      <c r="D34" s="11"/>
+      <c r="E34" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="F34" s="13" t="s">
+      <c r="F34" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="G34" s="11" t="s">
+      <c r="G34" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="H34" s="10"/>
+      <c r="H34" s="8"/>
     </row>
     <row r="35" spans="2:8" ht="36" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="12" t="s">
+      <c r="B35" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="C35" s="11" t="s">
+      <c r="C35" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D35" s="13"/>
-      <c r="E35" s="11" t="s">
+      <c r="D35" s="11"/>
+      <c r="E35" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="F35" s="13" t="s">
+      <c r="F35" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="G35" s="11" t="s">
+      <c r="G35" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="2:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" ht="36" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C39" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D39" s="14"/>
+      <c r="E39" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="F39" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G39" s="13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" ht="36" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D40" s="11"/>
+      <c r="E40" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="G40" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" ht="54" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C41" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D41" s="17"/>
+      <c r="E41" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="F41" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="G41" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" ht="54" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D42" s="11"/>
+      <c r="E42" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="F42" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="G42" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" ht="36" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D43" s="11"/>
+      <c r="E43" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="F43" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="G43" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" ht="36" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D44" s="11"/>
+      <c r="E44" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="F44" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="G44" s="9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" ht="53" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D45" s="11"/>
+      <c r="E45" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="F45" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="G45" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" ht="36" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D46" s="11"/>
+      <c r="E46" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="F46" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="G46" s="9" t="s">
         <v>66</v>
       </c>
     </row>

</xml_diff>

<commit_message>
request routes added and tested
</commit_message>
<xml_diff>
--- a/routes_design.xlsx
+++ b/routes_design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rumble/Documents/WeddingRequester/Function-Band-Request-a-Song-App/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDAB5425-3EB6-2449-9B3B-748D4D48FDA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A52C1216-6CF1-D040-907F-F79F92424DE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15800" xr2:uid="{D98520DE-90ED-1842-9CAD-02F5B5F8C61E}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="92">
   <si>
     <t>Route</t>
   </si>
@@ -517,6 +517,48 @@
   </si>
   <si>
     <t>/events/band_id/events</t>
+  </si>
+  <si>
+    <t>REQUESTS</t>
+  </si>
+  <si>
+    <t>/requests</t>
+  </si>
+  <si>
+    <t>/requests/{id}</t>
+  </si>
+  <si>
+    <t>Get request by request_id</t>
+  </si>
+  <si>
+    <t>request_id</t>
+  </si>
+  <si>
+    <t>JSON request object</t>
+  </si>
+  <si>
+    <t>Post a request</t>
+  </si>
+  <si>
+    <t>song_name, guest_id, event_id</t>
+  </si>
+  <si>
+    <t>JSON object and relevant response</t>
+  </si>
+  <si>
+    <t>Get all requests from an event</t>
+  </si>
+  <si>
+    <t>response array of request objects</t>
+  </si>
+  <si>
+    <t>Update a request</t>
+  </si>
+  <si>
+    <t>JSON response.</t>
+  </si>
+  <si>
+    <t>requests/event/&lt;int:event_id&gt;</t>
   </si>
 </sst>
 </file>
@@ -624,7 +666,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -675,6 +717,12 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -689,6 +737,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1003,10 +1059,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE3873A4-E976-7D46-8E74-B618A7E6E516}">
-  <dimension ref="B2:H46"/>
+  <dimension ref="B2:H56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1205,110 +1261,110 @@
       </c>
     </row>
     <row r="19" spans="2:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="19" t="s">
+      <c r="C19" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19" t="s">
+      <c r="D19" s="21"/>
+      <c r="E19" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="F19" s="19" t="s">
+      <c r="F19" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="G19" s="19" t="s">
+      <c r="G19" s="21" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="20" spans="2:8" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="21" t="s">
+      <c r="C20" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21" t="s">
+      <c r="D20" s="23"/>
+      <c r="E20" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="21" t="s">
+      <c r="F20" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="G20" s="21" t="s">
+      <c r="G20" s="23" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="21" spans="2:8" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="21" t="s">
+      <c r="C21" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21" t="s">
+      <c r="D21" s="23"/>
+      <c r="E21" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="F21" s="21" t="s">
+      <c r="F21" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="G21" s="21" t="s">
+      <c r="G21" s="23" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="22" spans="2:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="20" t="s">
+      <c r="B22" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="21" t="s">
+      <c r="C22" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21" t="s">
+      <c r="D22" s="23"/>
+      <c r="E22" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="F22" s="21" t="s">
+      <c r="F22" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="G22" s="21" t="s">
+      <c r="G22" s="23" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="23" spans="2:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="20" t="s">
+      <c r="B23" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="21" t="s">
+      <c r="C23" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21" t="s">
+      <c r="D23" s="23"/>
+      <c r="E23" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="F23" s="21" t="s">
+      <c r="F23" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="G23" s="21" t="s">
+      <c r="G23" s="23" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="24" spans="2:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="20" t="s">
+      <c r="B24" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="C24" s="18" t="s">
+      <c r="C24" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D24" s="22"/>
-      <c r="E24" s="19" t="s">
+      <c r="D24" s="24"/>
+      <c r="E24" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="F24" s="19" t="s">
+      <c r="F24" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="G24" s="23" t="s">
+      <c r="G24" s="25" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1660,6 +1716,120 @@
         <v>66</v>
       </c>
     </row>
+    <row r="48" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="49" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F50" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G50" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="C51" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D51" s="19"/>
+      <c r="E51" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="F51" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="G51" s="19" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="C52" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="D52" s="27"/>
+      <c r="E52" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="F52" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="G52" s="27" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="C53" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="D53" s="27"/>
+      <c r="E53" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="F53" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="G53" s="27" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="54" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="C54" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D54" s="27"/>
+      <c r="E54" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="F54" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="G54" s="27" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="55" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="26"/>
+      <c r="C55" s="27"/>
+      <c r="D55" s="27"/>
+      <c r="E55" s="27"/>
+      <c r="F55" s="27"/>
+      <c r="G55" s="27"/>
+    </row>
+    <row r="56" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="26"/>
+      <c r="C56" s="18"/>
+      <c r="D56" s="28"/>
+      <c r="E56" s="19"/>
+      <c r="F56" s="19"/>
+      <c r="G56" s="29"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated Routes Design Spreadsheet
</commit_message>
<xml_diff>
--- a/routes_design.xlsx
+++ b/routes_design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rumble/Documents/WeddingRequester/Function-Band-Request-a-Song-App/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A52C1216-6CF1-D040-907F-F79F92424DE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30D50D2C-0BDD-7848-8090-830B00D5A76B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15800" xr2:uid="{D98520DE-90ED-1842-9CAD-02F5B5F8C61E}"/>
   </bookViews>
@@ -588,7 +588,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -598,6 +598,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -666,7 +672,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -745,6 +751,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1061,8 +1079,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE3873A4-E976-7D46-8E74-B618A7E6E516}">
   <dimension ref="B2:H56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1743,74 +1761,74 @@
       </c>
     </row>
     <row r="51" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="18" t="s">
+      <c r="B51" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="C51" s="19" t="s">
+      <c r="C51" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="D51" s="19"/>
-      <c r="E51" s="19" t="s">
+      <c r="D51" s="31"/>
+      <c r="E51" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="F51" s="19" t="s">
+      <c r="F51" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="G51" s="19" t="s">
+      <c r="G51" s="31" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="52" spans="2:7" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="26" t="s">
+      <c r="B52" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="C52" s="27" t="s">
+      <c r="C52" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="D52" s="27"/>
-      <c r="E52" s="27" t="s">
+      <c r="D52" s="33"/>
+      <c r="E52" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="F52" s="27" t="s">
+      <c r="F52" s="33" t="s">
         <v>85</v>
       </c>
-      <c r="G52" s="27" t="s">
+      <c r="G52" s="33" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="53" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="26" t="s">
+      <c r="B53" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="C53" s="27" t="s">
+      <c r="C53" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="D53" s="27"/>
-      <c r="E53" s="27" t="s">
+      <c r="D53" s="33"/>
+      <c r="E53" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="F53" s="27" t="s">
+      <c r="F53" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="G53" s="27" t="s">
+      <c r="G53" s="33" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="54" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="26" t="s">
+      <c r="B54" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="C54" s="27" t="s">
+      <c r="C54" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="D54" s="27"/>
-      <c r="E54" s="27" t="s">
+      <c r="D54" s="33"/>
+      <c r="E54" s="33" t="s">
         <v>87</v>
       </c>
-      <c r="F54" s="27" t="s">
+      <c r="F54" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="G54" s="27" t="s">
+      <c r="G54" s="33" t="s">
         <v>88</v>
       </c>
     </row>

</xml_diff>

<commit_message>
flask templates and static directories setup, signupband and singupguest GET route added
</commit_message>
<xml_diff>
--- a/routes_design.xlsx
+++ b/routes_design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rumble/Documents/WeddingRequester/Function-Band-Request-a-Song-App/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30D50D2C-0BDD-7848-8090-830B00D5A76B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D084507B-4F93-9E45-B17B-07B84CAB9437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15800" xr2:uid="{D98520DE-90ED-1842-9CAD-02F5B5F8C61E}"/>
   </bookViews>
@@ -70,9 +70,6 @@
     <t>HTML</t>
   </si>
   <si>
-    <t>/signupuser</t>
-  </si>
-  <si>
     <t>POST</t>
   </si>
   <si>
@@ -559,6 +556,9 @@
   </si>
   <si>
     <t>requests/event/&lt;int:event_id&gt;</t>
+  </si>
+  <si>
+    <t>/signupguest</t>
   </si>
 </sst>
 </file>
@@ -672,7 +672,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -723,10 +723,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -743,14 +743,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1079,8 +1072,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE3873A4-E976-7D46-8E74-B618A7E6E516}">
   <dimension ref="B2:H56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="E65" sqref="E65"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1095,7 +1088,7 @@
     <row r="2" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
@@ -1139,7 +1132,7 @@
     <row r="7" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
@@ -1163,99 +1156,99 @@
       </c>
     </row>
     <row r="10" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="2" t="s">
+      <c r="B10" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="C10" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F10" s="2" t="s">
+      <c r="D10" s="30"/>
+      <c r="E10" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="30" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="G11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="2" t="s">
+    </row>
+    <row r="12" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="29" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="12" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F12" s="2" t="s">
+      <c r="D12" s="30"/>
+      <c r="E12" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G12" s="30" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="2:7" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="14" spans="2:7" ht="36" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" s="7" t="s">
         <v>39</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="16" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="17" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
@@ -1280,116 +1273,116 @@
     </row>
     <row r="19" spans="2:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C19" s="21" t="s">
         <v>7</v>
       </c>
       <c r="D19" s="21"/>
       <c r="E19" s="21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F19" s="21" t="s">
         <v>9</v>
       </c>
       <c r="G19" s="21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="2:8" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C20" s="23" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D20" s="23"/>
       <c r="E20" s="23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F20" s="23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G20" s="23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="2:8" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B21" s="22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C21" s="23" t="s">
         <v>7</v>
       </c>
       <c r="D21" s="23"/>
       <c r="E21" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="F21" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="F21" s="23" t="s">
-        <v>28</v>
-      </c>
       <c r="G21" s="23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="2:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B22" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="23" t="s">
         <v>25</v>
-      </c>
-      <c r="C22" s="23" t="s">
-        <v>26</v>
       </c>
       <c r="D22" s="23"/>
       <c r="E22" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="F22" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="G22" s="23" t="s">
         <v>31</v>
-      </c>
-      <c r="F22" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="G22" s="23" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="23" spans="2:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B23" s="22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C23" s="23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D23" s="23"/>
       <c r="E23" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="F23" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="G23" s="23" t="s">
         <v>34</v>
-      </c>
-      <c r="F23" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="G23" s="23" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="24" spans="2:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B24" s="22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C24" s="20" t="s">
         <v>7</v>
       </c>
       <c r="D24" s="24"/>
       <c r="E24" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="F24" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="F24" s="21" t="s">
+      <c r="G24" s="25" t="s">
         <v>75</v>
-      </c>
-      <c r="G24" s="25" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="25" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="26" spans="2:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27" spans="2:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
@@ -1415,159 +1408,159 @@
     </row>
     <row r="28" spans="2:8" ht="36" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C28" s="13" t="s">
         <v>7</v>
       </c>
       <c r="D28" s="14"/>
       <c r="E28" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F28" s="14" t="s">
         <v>9</v>
       </c>
       <c r="G28" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H28" s="8"/>
     </row>
     <row r="29" spans="2:8" ht="36" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C29" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D29" s="11"/>
       <c r="E29" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F29" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="F29" s="11" t="s">
+      <c r="G29" s="9" t="s">
         <v>47</v>
-      </c>
-      <c r="G29" s="9" t="s">
-        <v>48</v>
       </c>
       <c r="H29" s="8"/>
     </row>
     <row r="30" spans="2:8" ht="54" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D30" s="17"/>
       <c r="E30" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="F30" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="F30" s="17" t="s">
+      <c r="G30" s="16" t="s">
         <v>50</v>
-      </c>
-      <c r="G30" s="16" t="s">
-        <v>51</v>
       </c>
       <c r="H30" s="8"/>
     </row>
     <row r="31" spans="2:8" ht="54" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D31" s="11"/>
       <c r="E31" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="F31" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="F31" s="11" t="s">
+      <c r="G31" s="9" t="s">
         <v>53</v>
-      </c>
-      <c r="G31" s="9" t="s">
-        <v>54</v>
       </c>
       <c r="H31" s="8"/>
     </row>
     <row r="32" spans="2:8" ht="36" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D32" s="11"/>
       <c r="E32" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F32" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="G32" s="9" t="s">
         <v>55</v>
-      </c>
-      <c r="F32" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="G32" s="9" t="s">
-        <v>56</v>
       </c>
       <c r="H32" s="8"/>
     </row>
     <row r="33" spans="2:8" ht="36" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C33" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D33" s="11"/>
       <c r="E33" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F33" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="F33" s="11" t="s">
+      <c r="G33" s="9" t="s">
         <v>59</v>
-      </c>
-      <c r="G33" s="9" t="s">
-        <v>60</v>
       </c>
       <c r="H33" s="8"/>
     </row>
     <row r="34" spans="2:8" ht="53" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C34" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D34" s="11"/>
       <c r="E34" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F34" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="G34" s="9" t="s">
         <v>62</v>
-      </c>
-      <c r="F34" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="G34" s="9" t="s">
-        <v>63</v>
       </c>
       <c r="H34" s="8"/>
     </row>
     <row r="35" spans="2:8" ht="36" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C35" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D35" s="11"/>
       <c r="E35" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="F35" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="G35" s="9" t="s">
         <v>65</v>
-      </c>
-      <c r="F35" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="G35" s="9" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="36" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="37" spans="2:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B37" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="38" spans="2:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
@@ -1592,152 +1585,152 @@
     </row>
     <row r="39" spans="2:8" ht="36" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C39" s="13" t="s">
         <v>7</v>
       </c>
       <c r="D39" s="14"/>
       <c r="E39" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F39" s="14" t="s">
         <v>9</v>
       </c>
       <c r="G39" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="40" spans="2:8" ht="36" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B40" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C40" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D40" s="11"/>
       <c r="E40" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F40" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="F40" s="11" t="s">
+      <c r="G40" s="9" t="s">
         <v>47</v>
-      </c>
-      <c r="G40" s="9" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="41" spans="2:8" ht="54" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B41" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D41" s="17"/>
       <c r="E41" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="F41" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="F41" s="17" t="s">
+      <c r="G41" s="16" t="s">
         <v>50</v>
-      </c>
-      <c r="G41" s="16" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="42" spans="2:8" ht="54" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B42" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D42" s="11"/>
       <c r="E42" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="F42" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="F42" s="11" t="s">
+      <c r="G42" s="9" t="s">
         <v>53</v>
-      </c>
-      <c r="G42" s="9" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="43" spans="2:8" ht="36" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B43" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D43" s="11"/>
       <c r="E43" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F43" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="G43" s="9" t="s">
         <v>55</v>
-      </c>
-      <c r="F43" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="G43" s="9" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="44" spans="2:8" ht="36" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B44" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C44" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D44" s="11"/>
       <c r="E44" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F44" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="F44" s="11" t="s">
+      <c r="G44" s="9" t="s">
         <v>59</v>
-      </c>
-      <c r="G44" s="9" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="45" spans="2:8" ht="53" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C45" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D45" s="11"/>
       <c r="E45" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F45" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="G45" s="9" t="s">
         <v>62</v>
-      </c>
-      <c r="F45" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="G45" s="9" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="46" spans="2:8" ht="36" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C46" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D46" s="11"/>
       <c r="E46" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="F46" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="G46" s="9" t="s">
         <v>65</v>
-      </c>
-      <c r="F46" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="G46" s="9" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="48" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="49" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B49" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="50" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
@@ -1761,92 +1754,92 @@
       </c>
     </row>
     <row r="51" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="30" t="s">
+      <c r="B51" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="C51" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="D51" s="28"/>
+      <c r="E51" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="C51" s="31" t="s">
+      <c r="F51" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="G51" s="28" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="C52" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="D52" s="30"/>
+      <c r="E52" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="F52" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="G52" s="30" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="C53" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="D53" s="30"/>
+      <c r="E53" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="F53" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="G53" s="30" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="54" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="C54" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="D51" s="31"/>
-      <c r="E51" s="31" t="s">
-        <v>81</v>
-      </c>
-      <c r="F51" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="G51" s="31" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="52" spans="2:7" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="32" t="s">
-        <v>79</v>
-      </c>
-      <c r="C52" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="D52" s="33"/>
-      <c r="E52" s="33" t="s">
-        <v>84</v>
-      </c>
-      <c r="F52" s="33" t="s">
-        <v>85</v>
-      </c>
-      <c r="G52" s="33" t="s">
+      <c r="D54" s="30"/>
+      <c r="E54" s="30" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="53" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="C53" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="D53" s="33"/>
-      <c r="E53" s="33" t="s">
-        <v>89</v>
-      </c>
-      <c r="F53" s="33" t="s">
-        <v>82</v>
-      </c>
-      <c r="G53" s="33" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="54" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="32" t="s">
-        <v>91</v>
-      </c>
-      <c r="C54" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="D54" s="33"/>
-      <c r="E54" s="33" t="s">
+      <c r="F54" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="G54" s="30" t="s">
         <v>87</v>
       </c>
-      <c r="F54" s="33" t="s">
-        <v>28</v>
-      </c>
-      <c r="G54" s="33" t="s">
-        <v>88</v>
-      </c>
     </row>
     <row r="55" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="26"/>
-      <c r="C55" s="27"/>
-      <c r="D55" s="27"/>
-      <c r="E55" s="27"/>
-      <c r="F55" s="27"/>
-      <c r="G55" s="27"/>
+      <c r="B55" s="1"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
+      <c r="G55" s="2"/>
     </row>
     <row r="56" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="26"/>
+      <c r="B56" s="1"/>
       <c r="C56" s="18"/>
-      <c r="D56" s="28"/>
+      <c r="D56" s="5"/>
       <c r="E56" s="19"/>
       <c r="F56" s="19"/>
-      <c r="G56" s="29"/>
+      <c r="G56" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>